<commit_message>
fix a data bug
</commit_message>
<xml_diff>
--- a/expDatas.xlsx
+++ b/expDatas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19687\Desktop\Courses\Computer Science\Principes of Database System\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F67E439-3A92-483E-B19E-EF71A1800A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104D9684-C46F-4C72-9344-DF1BB851CE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loading" sheetId="1" r:id="rId1"/>
@@ -162,7 +162,7 @@
   <numFmts count="3">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="177" formatCode="0.0000_ "/>
-    <numFmt numFmtId="178" formatCode="0.0_ "/>
+    <numFmt numFmtId="179" formatCode="0.0000_);[Red]\(0.0000\)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -205,7 +205,7 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -350,19 +350,19 @@
             <c:numRef>
               <c:f>Loading!$E$2:$E$5</c:f>
               <c:numCache>
-                <c:formatCode>0.00_ </c:formatCode>
+                <c:formatCode>0.0000_);[Red]\(0.0000\)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>63232.333333333336</c:v>
+                  <c:v>0.79073469796570317</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>136486.66666666666</c:v>
+                  <c:v>3.6633615005128708</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>132003.66666666666</c:v>
+                  <c:v>3.787773571946234</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>126102.66666666667</c:v>
+                  <c:v>3.9650232086025143</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -536,7 +536,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" altLang="zh-CN"/>
-                  <a:t>time (ms)</a:t>
+                  <a:t>Inset</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+                  <a:t> speed</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t> (records/ms)</a:t>
                 </a:r>
                 <a:endParaRPr lang="zh-CN" altLang="en-US"/>
               </a:p>
@@ -571,7 +579,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00_ " sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000_);[Red]\(0.0000\)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2115,19 +2123,19 @@
             <c:numRef>
               <c:f>FInsert!$E$2:$E$5</c:f>
               <c:numCache>
-                <c:formatCode>0.0_ </c:formatCode>
+                <c:formatCode>0.0000_);[Red]\(0.0000\)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>63232.333333333336</c:v>
+                  <c:v>0.79073469796570317</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>136486.66666666666</c:v>
+                  <c:v>3.6633615005128708</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>132003.66666666666</c:v>
+                  <c:v>3.787773571946234</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>126102.66666666667</c:v>
+                  <c:v>3.9650232086025143</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2244,19 +2252,19 @@
             <c:numRef>
               <c:f>FInsert!$I$2:$I$5</c:f>
               <c:numCache>
-                <c:formatCode>0.0_ </c:formatCode>
+                <c:formatCode>0.0000_);[Red]\(0.0000\)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>62581</c:v>
+                  <c:v>0.79896454195362809</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18494</c:v>
+                  <c:v>27.035795393100464</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12542.666666666666</c:v>
+                  <c:v>39.863931115127038</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12127</c:v>
+                  <c:v>41.230312525768944</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2469,7 +2477,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.0_ " sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000_);[Red]\(0.0000\)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -11227,16 +11235,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11310,8 +11318,8 @@
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -11914,8 +11922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -11928,7 +11936,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -11945,9 +11953,9 @@
       <c r="D2">
         <v>67023</v>
       </c>
-      <c r="E2" s="1">
-        <f>AVERAGE(B2:D2)</f>
-        <v>63232.333333333336</v>
+      <c r="E2" s="4">
+        <f>50000/AVERAGE(B2:D2)</f>
+        <v>0.79073469796570317</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -11963,9 +11971,9 @@
       <c r="D3">
         <v>137013</v>
       </c>
-      <c r="E3" s="1">
-        <f t="shared" ref="E3:E5" si="0">AVERAGE(B3:D3)</f>
-        <v>136486.66666666666</v>
+      <c r="E3" s="4">
+        <f>500000/AVERAGE(B3:D3)</f>
+        <v>3.6633615005128708</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -11981,9 +11989,9 @@
       <c r="D4">
         <v>129523</v>
       </c>
-      <c r="E4" s="1">
-        <f t="shared" si="0"/>
-        <v>132003.66666666666</v>
+      <c r="E4" s="4">
+        <f>500000/AVERAGE(B4:D4)</f>
+        <v>3.787773571946234</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -11999,9 +12007,9 @@
       <c r="D5">
         <v>126070</v>
       </c>
-      <c r="E5" s="1">
-        <f t="shared" si="0"/>
-        <v>126102.66666666667</v>
+      <c r="E5" s="4">
+        <f>500000/AVERAGE(B5:D5)</f>
+        <v>3.9650232086025143</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -12044,7 +12052,7 @@
         <v>33.471699999999998</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" ref="E20:E26" si="1">AVERAGE(B20:D20)</f>
+        <f t="shared" ref="E20:E26" si="0">AVERAGE(B20:D20)</f>
         <v>35.151933333333332</v>
       </c>
     </row>
@@ -12062,7 +12070,7 @@
         <v>22.709700000000002</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>22.942233333333334</v>
       </c>
     </row>
@@ -12080,7 +12088,7 @@
         <v>35.456000000000003</v>
       </c>
       <c r="E22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>35.619633333333333</v>
       </c>
     </row>
@@ -12098,7 +12106,7 @@
         <v>30.0517</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>29.427066666666665</v>
       </c>
     </row>
@@ -12116,7 +12124,7 @@
         <v>29.935500000000001</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>29.444299999999998</v>
       </c>
     </row>
@@ -12134,7 +12142,7 @@
         <v>23.148099999999999</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>22.915233333333333</v>
       </c>
     </row>
@@ -12152,7 +12160,7 @@
         <v>35.890099999999997</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>36.350566666666658</v>
       </c>
     </row>
@@ -12167,24 +12175,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D0C87AB-2119-4448-9C19-63E59C0B7612}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.77734375" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -12202,8 +12211,8 @@
         <v>67023</v>
       </c>
       <c r="E2" s="4">
-        <f>AVERAGE(B2:D2)</f>
-        <v>63232.333333333336</v>
+        <f>50000/AVERAGE(B2:D2)</f>
+        <v>0.79073469796570317</v>
       </c>
       <c r="F2">
         <v>60337</v>
@@ -12215,8 +12224,8 @@
         <v>67229</v>
       </c>
       <c r="I2" s="4">
-        <f>AVERAGE(F2:H2)</f>
-        <v>62581</v>
+        <f>50000/AVERAGE(F2:H2)</f>
+        <v>0.79896454195362809</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -12233,8 +12242,8 @@
         <v>137013</v>
       </c>
       <c r="E3" s="4">
-        <f t="shared" ref="E3:E5" si="0">AVERAGE(B3:D3)</f>
-        <v>136486.66666666666</v>
+        <f>500000/AVERAGE(B3:D3)</f>
+        <v>3.6633615005128708</v>
       </c>
       <c r="F3">
         <v>18937</v>
@@ -12246,8 +12255,8 @@
         <v>17346</v>
       </c>
       <c r="I3" s="4">
-        <f t="shared" ref="I3:I5" si="1">AVERAGE(F3:H3)</f>
-        <v>18494</v>
+        <f>500000/AVERAGE(F3:H3)</f>
+        <v>27.035795393100464</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -12264,8 +12273,8 @@
         <v>129523</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" si="0"/>
-        <v>132003.66666666666</v>
+        <f>500000/AVERAGE(B4:D4)</f>
+        <v>3.787773571946234</v>
       </c>
       <c r="F4">
         <v>12636</v>
@@ -12277,8 +12286,8 @@
         <v>12496</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" si="1"/>
-        <v>12542.666666666666</v>
+        <f>500000/AVERAGE(F4:H4)</f>
+        <v>39.863931115127038</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -12295,8 +12304,8 @@
         <v>126070</v>
       </c>
       <c r="E5" s="4">
-        <f t="shared" si="0"/>
-        <v>126102.66666666667</v>
+        <f>500000/AVERAGE(B5:D5)</f>
+        <v>3.9650232086025143</v>
       </c>
       <c r="F5">
         <v>12343</v>
@@ -12308,8 +12317,8 @@
         <v>12154</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" si="1"/>
-        <v>12127</v>
+        <f>500000/AVERAGE(F5:H5)</f>
+        <v>41.230312525768944</v>
       </c>
     </row>
   </sheetData>
@@ -12795,7 +12804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C27390-B2BB-40BA-94B0-582B90E70529}">
   <dimension ref="A2:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>

</xml_diff>